<commit_message>
organize baseline rides import
</commit_message>
<xml_diff>
--- a/Replication Package/documentation/rider-audits/baseline-study/codebooks/raw.xlsx
+++ b/Replication Package/documentation/rider-audits/baseline-study/codebooks/raw.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb501238\Documents\GitHub\rio_vagao_rosa\documentation\rider-audits\baseline-study\codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb501238\Documents\GitHub\rio-safe-space\Replication Package\documentation\rider-audits\baseline-study\codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F839BD-51AD-400E-84B1-82F2D0F0CAA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F062CF-F9C4-4441-A8FF-6DAEFEEC9B55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="227">
   <si>
     <t>name</t>
   </si>
@@ -711,15 +711,6 @@
   </si>
   <si>
     <t>Unique ride ID</t>
-  </si>
-  <si>
-    <t>drop_user</t>
-  </si>
-  <si>
-    <t>user_gender_corr</t>
-  </si>
-  <si>
-    <t>demo_merge</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I153"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="E157" sqref="E157"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5020,21 +5011,6 @@
       </c>
       <c r="I150" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9">
-      <c r="E151" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9">
-      <c r="E152" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9">
-      <c r="E153" t="s">
-        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>